<commit_message>
Powerboard V3, Notes in the logbook
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bergg\PCBs\rover-hardware\Logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF170FA-2560-41A3-9AAE-BA766762A880}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD5BF70-60B0-480E-BA18-ECBFE149FC0D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4080" xr2:uid="{4CBD3E50-7A53-4B21-9737-B74C9B8148FB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t xml:space="preserve">Tested for Transistor types </t>
+  </si>
+  <si>
+    <t>Completed the Batt output with 2N3906 transistor in it.</t>
+  </si>
+  <si>
+    <t>Added 2N3906 transistor Datasheet to components file</t>
   </si>
 </sst>
 </file>
@@ -63,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -85,6 +91,17 @@
       <right style="thick">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top style="thick">
         <color auto="1"/>
       </top>
@@ -92,19 +109,89 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thick">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -115,7 +202,18 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -127,32 +225,8 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -161,18 +235,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,16 +567,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F5C064-8CD5-4D4D-865E-F5EACD682F22}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -504,36 +584,86 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="9">
         <v>43162</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
+        <v>43166</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="16"/>
+      <c r="B6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to High Power Circuit
Added a bunch of changes that can be seen on the change log
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28016"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bergg\PCBs\rover-hardware\Logbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/Logbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD5BF70-60B0-480E-BA18-ECBFE149FC0D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4080" xr2:uid="{4CBD3E50-7A53-4B21-9737-B74C9B8148FB}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -47,11 +52,14 @@
   <si>
     <t>Added 2N3906 transistor Datasheet to components file</t>
   </si>
+  <si>
+    <t>Created High Power Circuit and added terminal blocks, power supply, motor controller terminal blocks, and battery input</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -253,6 +261,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,16 +592,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F5C064-8CD5-4D4D-865E-F5EACD682F22}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -591,7 +617,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>43162</v>
       </c>
@@ -607,7 +633,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -621,7 +647,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -635,7 +661,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>43166</v>
       </c>
@@ -651,7 +677,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="14" t="s">
         <v>6</v>
@@ -665,7 +691,38 @@
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>43167</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B7:J8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added changes to LowPowerSchematic
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Created High Power Circuit and added terminal blocks, power supply, motor controller terminal blocks, and battery input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added SENSE_R global variable to sense resistor circuit. Changed BJTs to MOSFET equivalents. Also added text, descriptions for different blocks of circuit. </t>
   </si>
 </sst>
 </file>
@@ -593,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -719,9 +722,38 @@
       <c r="I8" s="21"/>
       <c r="J8" s="22"/>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>43167</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B7:J8"/>
+    <mergeCell ref="B9:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed DSH to DSG and added initials to logs
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28016"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/Logbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bergg\PCBs\rover-hardware\Logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB471EBC-4066-4D00-9F89-9083E11782CC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -57,12 +58,18 @@
   </si>
   <si>
     <t xml:space="preserve">Added SENSE_R global variable to sense resistor circuit. Changed BJTs to MOSFET equivalents. Also added text, descriptions for different blocks of circuit. </t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>TS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -595,16 +602,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -620,7 +627,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>43162</v>
       </c>
@@ -636,8 +643,10 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -650,7 +659,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -664,7 +673,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>43166</v>
       </c>
@@ -680,8 +689,10 @@
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="B6" s="14" t="s">
         <v>6</v>
       </c>
@@ -694,7 +705,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>43167</v>
       </c>
@@ -710,8 +721,10 @@
       <c r="I7" s="18"/>
       <c r="J7" s="19"/>
     </row>
-    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
@@ -722,7 +735,7 @@
       <c r="I8" s="21"/>
       <c r="J8" s="22"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>43167</v>
       </c>
@@ -738,8 +751,10 @@
       <c r="I9" s="18"/>
       <c r="J9" s="19"/>
     </row>
-    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="B10" s="20"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>

</xml_diff>

<commit_message>
Worked on LPC, More infor in Log
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bergg\PCBs\rover-hardware\Logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB471EBC-4066-4D00-9F89-9083E11782CC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B28B374-BCD5-429E-BD83-9CBAF85E8972}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>TS</t>
+  </si>
+  <si>
+    <t>Finsihed Battery Management IC Connections and Double Checked them.</t>
+  </si>
+  <si>
+    <t>Added information on Microcontroller Inputs.</t>
+  </si>
+  <si>
+    <t>Posted question underneath High Power Circuit.</t>
   </si>
 </sst>
 </file>
@@ -87,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -247,13 +256,59 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -289,6 +344,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,6 +824,52 @@
       <c r="I10" s="21"/>
       <c r="J10" s="22"/>
     </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="23">
+        <v>43168</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="25"/>
+      <c r="B13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B7:J8"/>

</xml_diff>

<commit_message>
Deleted Barrel Jack Connectors
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/Logbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79115676-AD66-A642-82D6-DF336B5044A2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC79CE0D-8A5D-8641-AB0E-BFF6B8E714FD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Removed connection between BATT- and GND. Had to replace BATT- with GND on some 24V terminal Blocks.</t>
+  </si>
+  <si>
+    <t>Deleted Barrel jack 12V power connections after talking to Carl. Deemed unecessary.</t>
   </si>
 </sst>
 </file>
@@ -671,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:J19"/>
+      <selection activeCell="B20" sqref="B20:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -969,8 +972,39 @@
       <c r="I19" s="25"/>
       <c r="J19" s="26"/>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>43170</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B20:J21"/>
     <mergeCell ref="B7:J8"/>
     <mergeCell ref="B9:J10"/>
     <mergeCell ref="B14:J15"/>

</xml_diff>

<commit_message>
Added info to logbook
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\codyb\USST\rover-hardware\Logbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/Logbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0D3D4A-1B14-441D-9627-D843C113E279}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073615D8-EB2F-1644-A784-52B7B90699FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">pcb board. Added the IRF3205 transistor to the BOM. </t>
+  </si>
+  <si>
+    <t>Moved a bunch of things around and started placing tracks</t>
   </si>
 </sst>
 </file>
@@ -348,6 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -366,7 +370,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,15 +684,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:A23"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -705,7 +708,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>43162</v>
       </c>
@@ -721,7 +724,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -737,7 +740,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -751,7 +754,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>43166</v>
       </c>
@@ -767,7 +770,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -783,67 +786,67 @@
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>43167</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="24"/>
+    </row>
+    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>43167</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="24"/>
+    </row>
+    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>43168</v>
       </c>
@@ -859,7 +862,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>9</v>
       </c>
@@ -875,7 +878,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="14" t="s">
         <v>13</v>
@@ -889,127 +892,127 @@
       <c r="I13" s="12"/>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>43168</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="24"/>
+    </row>
+    <row r="15" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="26"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>43169</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="24"/>
+    </row>
+    <row r="17" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="26"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>43170</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
-    </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="24"/>
+    </row>
+    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="26"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>43170</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="23"/>
-    </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="24"/>
+    </row>
+    <row r="21" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="26"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="27"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <v>43180</v>
       </c>
@@ -1025,11 +1028,11 @@
       <c r="I22" s="7"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="12"/>
@@ -1041,8 +1044,39 @@
       <c r="I23" s="12"/>
       <c r="J23" s="13"/>
     </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>43170</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="24"/>
+    </row>
+    <row r="25" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B24:J25"/>
     <mergeCell ref="B20:J21"/>
     <mergeCell ref="B7:J8"/>
     <mergeCell ref="B9:J10"/>

</xml_diff>

<commit_message>
Finsished Pcbnew PowerBoard V3. Needs to be checked
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/Logbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\codyb\USST\rover-hardware\Logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5549BE79-69B2-E949-A4A7-767209E65B2F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0F807F-E96B-41E7-B963-F22BEFB813D4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t xml:space="preserve">Changed the location of many terminal blocks after discussion with Tyrel. Also started making proper track sizing for the larger amperages. Removed the 3.3V terminal block as 3.3V will not be used anywhere within the box. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finished the PowerBoardV3. It reads zero errors from the DRC (ladybug) test. Needs to be double checked for trace widths, etc. </t>
   </si>
 </sst>
 </file>
@@ -376,6 +379,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -392,24 +413,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -732,18 +735,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A30:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -759,7 +762,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>43162</v>
       </c>
@@ -775,7 +778,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -791,7 +794,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -805,7 +808,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>43166</v>
       </c>
@@ -821,7 +824,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -837,67 +840,67 @@
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>43167</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="29"/>
-    </row>
-    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="24"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>43167</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
-    </row>
-    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="24"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="17">
         <v>43168</v>
       </c>
@@ -913,7 +916,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>9</v>
       </c>
@@ -929,7 +932,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="19"/>
       <c r="B13" s="14" t="s">
         <v>13</v>
@@ -943,248 +946,279 @@
       <c r="I13" s="12"/>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>43168</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="29"/>
-    </row>
-    <row r="15" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="23"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="32"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>43169</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="29"/>
-    </row>
-    <row r="17" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="32"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>43170</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="29"/>
-    </row>
-    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="23"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="32"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>43170</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="29"/>
-    </row>
-    <row r="21" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="32"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="24"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="26"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="17">
         <v>43180</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
       <c r="J22" s="33"/>
     </row>
-    <row r="23" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
       <c r="J23" s="34"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>43183</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="29"/>
-    </row>
-    <row r="25" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="23"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="32"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="17">
         <v>43187</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="23"/>
-    </row>
-    <row r="27" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="29"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="26"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="30"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="32"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="17">
         <v>43190</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="29"/>
-    </row>
-    <row r="29" spans="1:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="23"/>
+    </row>
+    <row r="29" spans="1:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="26"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="17">
+        <v>43194</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="29"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B30:J31"/>
     <mergeCell ref="B28:J29"/>
     <mergeCell ref="B26:J27"/>
     <mergeCell ref="B24:J25"/>

</xml_diff>

<commit_message>
A lot of changes following realization of thickness constraints
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/Logbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC43748F-3808-C74F-9848-E20AD95DDB5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5D6FE6-3EA2-C542-A536-A44F1E13EDB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -102,7 +102,7 @@
     <t xml:space="preserve">Finished the PowerBoardV3. It reads zero errors from the DRC (ladybug) test. Needs to be double checked for trace widths, etc. </t>
   </si>
   <si>
-    <t>Added footprint for vertical battery input connector and added four cm to the top of the cutout.</t>
+    <t>Added footprint for vertical battery input connector and added four cm to the top of the cutout. Completely Changed the thicknesses. Used areas instead.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fixed errors on PowerBoardV3
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/Logbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\codyb\USST\rover-hardware\Logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5D6FE6-3EA2-C542-A536-A44F1E13EDB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF45C56-3940-4429-A328-95FD95F67385}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Added footprint for vertical battery input connector and added four cm to the top of the cutout. Completely Changed the thicknesses. Used areas instead.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleaned up errors. </t>
   </si>
 </sst>
 </file>
@@ -738,18 +741,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:J33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -765,7 +768,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="9">
         <v>43162</v>
       </c>
@@ -781,7 +784,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -797,7 +800,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -811,7 +814,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="9">
         <v>43166</v>
       </c>
@@ -827,7 +830,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -843,7 +846,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <v>43167</v>
       </c>
@@ -859,7 +862,7 @@
       <c r="I7" s="28"/>
       <c r="J7" s="29"/>
     </row>
-    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
@@ -873,7 +876,7 @@
       <c r="I8" s="31"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <v>43167</v>
       </c>
@@ -889,7 +892,7 @@
       <c r="I9" s="28"/>
       <c r="J9" s="29"/>
     </row>
-    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
@@ -903,7 +906,7 @@
       <c r="I10" s="31"/>
       <c r="J10" s="32"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="17">
         <v>43168</v>
       </c>
@@ -919,7 +922,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>9</v>
       </c>
@@ -935,7 +938,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="19"/>
       <c r="B13" s="14" t="s">
         <v>13</v>
@@ -949,7 +952,7 @@
       <c r="I13" s="12"/>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="9">
         <v>43168</v>
       </c>
@@ -965,7 +968,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="29"/>
     </row>
-    <row r="15" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="16" t="s">
         <v>10</v>
       </c>
@@ -979,7 +982,7 @@
       <c r="I15" s="31"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="9">
         <v>43169</v>
       </c>
@@ -995,7 +998,7 @@
       <c r="I16" s="28"/>
       <c r="J16" s="29"/>
     </row>
-    <row r="17" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="16" t="s">
         <v>10</v>
       </c>
@@ -1009,7 +1012,7 @@
       <c r="I17" s="31"/>
       <c r="J17" s="32"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="9">
         <v>43170</v>
       </c>
@@ -1025,7 +1028,7 @@
       <c r="I18" s="28"/>
       <c r="J18" s="29"/>
     </row>
-    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
@@ -1039,7 +1042,7 @@
       <c r="I19" s="31"/>
       <c r="J19" s="32"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="9">
         <v>43170</v>
       </c>
@@ -1055,7 +1058,7 @@
       <c r="I20" s="28"/>
       <c r="J20" s="29"/>
     </row>
-    <row r="21" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="16" t="s">
         <v>10</v>
       </c>
@@ -1069,7 +1072,7 @@
       <c r="I21" s="31"/>
       <c r="J21" s="32"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="17">
         <v>43180</v>
       </c>
@@ -1085,7 +1088,7 @@
       <c r="I22" s="22"/>
       <c r="J22" s="33"/>
     </row>
-    <row r="23" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="19" t="s">
         <v>9</v>
       </c>
@@ -1099,7 +1102,7 @@
       <c r="I23" s="25"/>
       <c r="J23" s="34"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="9">
         <v>43183</v>
       </c>
@@ -1115,7 +1118,7 @@
       <c r="I24" s="28"/>
       <c r="J24" s="29"/>
     </row>
-    <row r="25" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="16" t="s">
         <v>10</v>
       </c>
@@ -1129,7 +1132,7 @@
       <c r="I25" s="31"/>
       <c r="J25" s="32"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="17">
         <v>43187</v>
       </c>
@@ -1145,7 +1148,7 @@
       <c r="I26" s="22"/>
       <c r="J26" s="23"/>
     </row>
-    <row r="27" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="19" t="s">
         <v>9</v>
       </c>
@@ -1159,7 +1162,7 @@
       <c r="I27" s="25"/>
       <c r="J27" s="26"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="17">
         <v>43190</v>
       </c>
@@ -1175,7 +1178,7 @@
       <c r="I28" s="28"/>
       <c r="J28" s="29"/>
     </row>
-    <row r="29" spans="1:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="16" t="s">
         <v>10</v>
       </c>
@@ -1189,7 +1192,7 @@
       <c r="I29" s="31"/>
       <c r="J29" s="32"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="17">
         <v>43194</v>
       </c>
@@ -1205,7 +1208,7 @@
       <c r="I30" s="22"/>
       <c r="J30" s="23"/>
     </row>
-    <row r="31" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="19" t="s">
         <v>9</v>
       </c>
@@ -1219,7 +1222,7 @@
       <c r="I31" s="25"/>
       <c r="J31" s="26"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="17">
         <v>43199</v>
       </c>
@@ -1235,7 +1238,7 @@
       <c r="I32" s="22"/>
       <c r="J32" s="23"/>
     </row>
-    <row r="33" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="19" t="s">
         <v>10</v>
       </c>
@@ -1249,8 +1252,39 @@
       <c r="I33" s="25"/>
       <c r="J33" s="26"/>
     </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" s="17">
+        <v>43206</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="23"/>
+    </row>
+    <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="B34:J35"/>
     <mergeCell ref="B32:J33"/>
     <mergeCell ref="B7:J8"/>
     <mergeCell ref="B9:J10"/>

</xml_diff>

<commit_message>
Made the Arm PCB
</commit_message>
<xml_diff>
--- a/Logbooks/PowerBoard V3 Logbook.xlsx
+++ b/Logbooks/PowerBoard V3 Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\codyb\USST\rover-hardware\Logbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/Logbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF45C56-3940-4429-A328-95FD95F67385}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA17426-561F-AC40-BF89-F6F240A22D43}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cleaned up errors. </t>
+  </si>
+  <si>
+    <t>Created Arm power board pcb with all parts</t>
   </si>
 </sst>
 </file>
@@ -741,18 +744,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -768,7 +771,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="11"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>43162</v>
       </c>
@@ -784,7 +787,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -800,7 +803,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -814,7 +817,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>43166</v>
       </c>
@@ -830,7 +833,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -846,7 +849,7 @@
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>43167</v>
       </c>
@@ -862,7 +865,7 @@
       <c r="I7" s="28"/>
       <c r="J7" s="29"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
@@ -876,7 +879,7 @@
       <c r="I8" s="31"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>43167</v>
       </c>
@@ -892,7 +895,7 @@
       <c r="I9" s="28"/>
       <c r="J9" s="29"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
@@ -906,7 +909,7 @@
       <c r="I10" s="31"/>
       <c r="J10" s="32"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="17">
         <v>43168</v>
       </c>
@@ -922,7 +925,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>9</v>
       </c>
@@ -938,7 +941,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="14" t="s">
         <v>13</v>
@@ -952,7 +955,7 @@
       <c r="I13" s="12"/>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>43168</v>
       </c>
@@ -968,7 +971,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="29"/>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>10</v>
       </c>
@@ -982,7 +985,7 @@
       <c r="I15" s="31"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>43169</v>
       </c>
@@ -998,7 +1001,7 @@
       <c r="I16" s="28"/>
       <c r="J16" s="29"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>10</v>
       </c>
@@ -1012,7 +1015,7 @@
       <c r="I17" s="31"/>
       <c r="J17" s="32"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>43170</v>
       </c>
@@ -1028,7 +1031,7 @@
       <c r="I18" s="28"/>
       <c r="J18" s="29"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
@@ -1042,7 +1045,7 @@
       <c r="I19" s="31"/>
       <c r="J19" s="32"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>43170</v>
       </c>
@@ -1058,7 +1061,7 @@
       <c r="I20" s="28"/>
       <c r="J20" s="29"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>10</v>
       </c>
@@ -1072,7 +1075,7 @@
       <c r="I21" s="31"/>
       <c r="J21" s="32"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="17">
         <v>43180</v>
       </c>
@@ -1088,7 +1091,7 @@
       <c r="I22" s="22"/>
       <c r="J22" s="33"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>9</v>
       </c>
@@ -1102,7 +1105,7 @@
       <c r="I23" s="25"/>
       <c r="J23" s="34"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>43183</v>
       </c>
@@ -1118,7 +1121,7 @@
       <c r="I24" s="28"/>
       <c r="J24" s="29"/>
     </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>10</v>
       </c>
@@ -1132,7 +1135,7 @@
       <c r="I25" s="31"/>
       <c r="J25" s="32"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="17">
         <v>43187</v>
       </c>
@@ -1148,7 +1151,7 @@
       <c r="I26" s="22"/>
       <c r="J26" s="23"/>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>9</v>
       </c>
@@ -1162,7 +1165,7 @@
       <c r="I27" s="25"/>
       <c r="J27" s="26"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="17">
         <v>43190</v>
       </c>
@@ -1178,7 +1181,7 @@
       <c r="I28" s="28"/>
       <c r="J28" s="29"/>
     </row>
-    <row r="29" spans="1:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>10</v>
       </c>
@@ -1192,7 +1195,7 @@
       <c r="I29" s="31"/>
       <c r="J29" s="32"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="17">
         <v>43194</v>
       </c>
@@ -1208,7 +1211,7 @@
       <c r="I30" s="22"/>
       <c r="J30" s="23"/>
     </row>
-    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
         <v>9</v>
       </c>
@@ -1222,7 +1225,7 @@
       <c r="I31" s="25"/>
       <c r="J31" s="26"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="17">
         <v>43199</v>
       </c>
@@ -1238,7 +1241,7 @@
       <c r="I32" s="22"/>
       <c r="J32" s="23"/>
     </row>
-    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>10</v>
       </c>
@@ -1252,7 +1255,7 @@
       <c r="I33" s="25"/>
       <c r="J33" s="26"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="17">
         <v>43206</v>
       </c>
@@ -1268,7 +1271,7 @@
       <c r="I34" s="22"/>
       <c r="J34" s="23"/>
     </row>
-    <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>9</v>
       </c>
@@ -1282,8 +1285,39 @@
       <c r="I35" s="25"/>
       <c r="J35" s="26"/>
     </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="17">
+        <v>43215</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="23"/>
+    </row>
+    <row r="37" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="B36:J37"/>
     <mergeCell ref="B34:J35"/>
     <mergeCell ref="B32:J33"/>
     <mergeCell ref="B7:J8"/>

</xml_diff>